<commit_message>
Location ar jonno alada db table
</commit_message>
<xml_diff>
--- a/Ollo_InventorySystem/VendorFiles/MkLteRoutersProperFormat.xlsx
+++ b/Ollo_InventorySystem/VendorFiles/MkLteRoutersProperFormat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="112">
   <si>
     <t>Item-Code</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t xml:space="preserve">LTE </t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>WareHouse</t>
   </si>
 </sst>
 </file>
@@ -681,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,9 +700,10 @@
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -718,8 +725,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -741,8 +751,11 @@
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -764,8 +777,11 @@
       <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -787,8 +803,11 @@
       <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -810,8 +829,11 @@
       <c r="G5" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -833,8 +855,11 @@
       <c r="G6" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -856,8 +881,11 @@
       <c r="G7" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -879,8 +907,11 @@
       <c r="G8" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -902,8 +933,11 @@
       <c r="G9" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -925,8 +959,11 @@
       <c r="G10" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -948,8 +985,11 @@
       <c r="G11" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -971,8 +1011,11 @@
       <c r="G12" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -994,8 +1037,11 @@
       <c r="G13" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1017,8 +1063,11 @@
       <c r="G14" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1040,8 +1089,11 @@
       <c r="G15" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1063,8 +1115,11 @@
       <c r="G16" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1086,8 +1141,11 @@
       <c r="G17" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1109,8 +1167,11 @@
       <c r="G18" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1132,8 +1193,11 @@
       <c r="G19" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1155,8 +1219,11 @@
       <c r="G20" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1178,8 +1245,11 @@
       <c r="G21" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1201,8 +1271,11 @@
       <c r="G22" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1224,8 +1297,11 @@
       <c r="G23" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1247,8 +1323,11 @@
       <c r="G24" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1270,8 +1349,11 @@
       <c r="G25" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1292,6 +1374,9 @@
       </c>
       <c r="G26" s="2" t="s">
         <v>108</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>